<commit_message>
+ cuota asamblea organizada
</commit_message>
<xml_diff>
--- a/Datos/Cuota_Asamblea_maportes.xlsx
+++ b/Datos/Cuota_Asamblea_maportes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7200" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7200" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cuota_Asamblea" sheetId="1" r:id="rId1"/>
@@ -968,9 +968,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1400,8 +1398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K411"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
@@ -15802,9 +15800,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>